<commit_message>
Webserver basado en ficheros html
Cambios:
-Las paginas web se leen desde el SPIFFS en lugar de generarlas dinamicamente
</commit_message>
<xml_diff>
--- a/MapaHoras.xlsx
+++ b/MapaHoras.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\arduino\desarrollos\Sketchs\Termostato\Codigo\ControladorM5s\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EB2702-6F37-4F5C-BA62-F48A0F47D870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863AB57B-3713-43C7-A359-C24C74D49FFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="66">
   <si>
     <t>Lunes</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t xml:space="preserve">  "</t>
+  </si>
+  <si>
+    <t>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127</t>
   </si>
 </sst>
 </file>
@@ -26588,10 +26591,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D608A227-2FCC-426A-81C3-15B0DED7161C}">
-  <dimension ref="B1:U50"/>
+  <dimension ref="B1:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA27" sqref="AA27"/>
+    <sheetView tabSelected="1" topLeftCell="I26" workbookViewId="0">
+      <selection activeCell="AA51" sqref="AA51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26610,7 +26613,7 @@
     <col min="22" max="36" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
@@ -26642,7 +26645,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B2" s="17">
         <v>0</v>
       </c>
@@ -26671,7 +26674,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="9">
-        <f>1*C2+2*D2+4*E2+8*F2+16*G2+32*H2+64*I2+128*J2</f>
+        <f t="shared" ref="K2:K49" si="0">1*C2+2*D2+4*E2+8*F2+16*G2+32*H2+64*I2+128*J2</f>
         <v>0</v>
       </c>
       <c r="O2" t="s">
@@ -26684,7 +26687,7 @@
         <v>13</v>
       </c>
       <c r="R2">
-        <f>+K2</f>
+        <f t="shared" ref="R2:R49" si="1">+K2</f>
         <v>0</v>
       </c>
       <c r="S2" t="s">
@@ -26694,8 +26697,16 @@
         <f>+CONCATENATE(O2,P2,Q2,R2,S2)</f>
         <v xml:space="preserve">  "0000":"0",</v>
       </c>
+      <c r="Y2">
+        <f>+R2</f>
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <f>+Y2</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" s="18">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -26724,7 +26735,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="4">
-        <f>1*C3+2*D3+4*E3+8*F3+16*G3+32*H3+64*I3+128*J3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O3" t="s">
@@ -26737,18 +26748,26 @@
         <v>13</v>
       </c>
       <c r="R3">
-        <f>+K3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S3" t="s">
         <v>12</v>
       </c>
       <c r="U3" s="21" t="str">
-        <f t="shared" ref="U3:U49" si="0">+CONCATENATE(O3,P3,Q3,R3,S3)</f>
+        <f t="shared" ref="U3:U49" si="2">+CONCATENATE(O3,P3,Q3,R3,S3)</f>
         <v xml:space="preserve">  "0030":"0",</v>
       </c>
+      <c r="Y3">
+        <f t="shared" ref="Y3:Y49" si="3">+R3</f>
+        <v>0</v>
+      </c>
+      <c r="AA3" t="str">
+        <f>+CONCATENATE(AA2,"|",Y3)</f>
+        <v>0|0</v>
+      </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" s="19">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -26777,7 +26796,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="5">
-        <f>1*C4+2*D4+4*E4+8*F4+16*G4+32*H4+64*I4+128*J4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O4" t="s">
@@ -26790,18 +26809,26 @@
         <v>13</v>
       </c>
       <c r="R4">
-        <f>+K4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S4" t="s">
         <v>12</v>
       </c>
       <c r="U4" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0100":"0",</v>
       </c>
+      <c r="Y4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA4" t="str">
+        <f t="shared" ref="AA4:AA49" si="4">+CONCATENATE(AA3,"|",Y4)</f>
+        <v>0|0|0</v>
+      </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B5" s="18">
         <v>6.25E-2</v>
       </c>
@@ -26830,7 +26857,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="4">
-        <f>1*C5+2*D5+4*E5+8*F5+16*G5+32*H5+64*I5+128*J5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O5" t="s">
@@ -26843,18 +26870,26 @@
         <v>13</v>
       </c>
       <c r="R5">
-        <f>+K5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S5" t="s">
         <v>12</v>
       </c>
       <c r="U5" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0130":"0",</v>
       </c>
+      <c r="Y5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA5" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0</v>
+      </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6" s="19">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -26883,7 +26918,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="5">
-        <f>1*C6+2*D6+4*E6+8*F6+16*G6+32*H6+64*I6+128*J6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O6" t="s">
@@ -26896,18 +26931,26 @@
         <v>13</v>
       </c>
       <c r="R6">
-        <f>+K6</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S6" t="s">
         <v>12</v>
       </c>
       <c r="U6" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0200":"0",</v>
       </c>
+      <c r="Y6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA6" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0</v>
+      </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B7" s="18">
         <v>0.104166666666667</v>
       </c>
@@ -26936,7 +26979,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="4">
-        <f>1*C7+2*D7+4*E7+8*F7+16*G7+32*H7+64*I7+128*J7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O7" t="s">
@@ -26949,18 +26992,26 @@
         <v>13</v>
       </c>
       <c r="R7">
-        <f>+K7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S7" t="s">
         <v>12</v>
       </c>
       <c r="U7" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0230":"0",</v>
       </c>
+      <c r="Y7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA7" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0</v>
+      </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B8" s="19">
         <v>0.125</v>
       </c>
@@ -26989,7 +27040,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="5">
-        <f>1*C8+2*D8+4*E8+8*F8+16*G8+32*H8+64*I8+128*J8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O8" t="s">
@@ -27002,18 +27053,26 @@
         <v>13</v>
       </c>
       <c r="R8">
-        <f>+K8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S8" t="s">
         <v>12</v>
       </c>
       <c r="U8" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0300":"0",</v>
       </c>
+      <c r="Y8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0</v>
+      </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B9" s="18">
         <v>0.14583333333333301</v>
       </c>
@@ -27042,7 +27101,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="4">
-        <f>1*C9+2*D9+4*E9+8*F9+16*G9+32*H9+64*I9+128*J9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O9" t="s">
@@ -27055,18 +27114,26 @@
         <v>13</v>
       </c>
       <c r="R9">
-        <f>+K9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S9" t="s">
         <v>12</v>
       </c>
       <c r="U9" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0330":"0",</v>
       </c>
+      <c r="Y9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA9" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0</v>
+      </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B10" s="19">
         <v>0.16666666666666699</v>
       </c>
@@ -27095,7 +27162,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="5">
-        <f>1*C10+2*D10+4*E10+8*F10+16*G10+32*H10+64*I10+128*J10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O10" t="s">
@@ -27108,18 +27175,26 @@
         <v>13</v>
       </c>
       <c r="R10">
-        <f>+K10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S10" t="s">
         <v>12</v>
       </c>
       <c r="U10" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0400":"0",</v>
       </c>
+      <c r="Y10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA10" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0</v>
+      </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B11" s="18">
         <v>0.1875</v>
       </c>
@@ -27148,7 +27223,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="4">
-        <f>1*C11+2*D11+4*E11+8*F11+16*G11+32*H11+64*I11+128*J11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O11" t="s">
@@ -27161,18 +27236,26 @@
         <v>13</v>
       </c>
       <c r="R11">
-        <f>+K11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S11" t="s">
         <v>12</v>
       </c>
       <c r="U11" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0430":"0",</v>
       </c>
+      <c r="Y11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA11" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0</v>
+      </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B12" s="19">
         <v>0.20833333333333301</v>
       </c>
@@ -27201,7 +27284,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="5">
-        <f>1*C12+2*D12+4*E12+8*F12+16*G12+32*H12+64*I12+128*J12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O12" t="s">
@@ -27214,18 +27297,26 @@
         <v>13</v>
       </c>
       <c r="R12">
-        <f>+K12</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S12" t="s">
         <v>12</v>
       </c>
       <c r="U12" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0500":"0",</v>
       </c>
+      <c r="Y12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA12" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0</v>
+      </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B13" s="18">
         <v>0.22916666666666699</v>
       </c>
@@ -27254,7 +27345,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="4">
-        <f>1*C13+2*D13+4*E13+8*F13+16*G13+32*H13+64*I13+128*J13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O13" t="s">
@@ -27267,18 +27358,26 @@
         <v>13</v>
       </c>
       <c r="R13">
-        <f>+K13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S13" t="s">
         <v>12</v>
       </c>
       <c r="U13" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0530":"0",</v>
       </c>
+      <c r="Y13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA13" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0</v>
+      </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B14" s="19">
         <v>0.25</v>
       </c>
@@ -27307,7 +27406,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="5">
-        <f>1*C14+2*D14+4*E14+8*F14+16*G14+32*H14+64*I14+128*J14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O14" t="s">
@@ -27320,18 +27419,26 @@
         <v>13</v>
       </c>
       <c r="R14">
-        <f>+K14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S14" t="s">
         <v>12</v>
       </c>
       <c r="U14" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0600":"0",</v>
       </c>
+      <c r="Y14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA14" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0</v>
+      </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B15" s="18">
         <v>0.27083333333333298</v>
       </c>
@@ -27360,7 +27467,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="4">
-        <f>1*C15+2*D15+4*E15+8*F15+16*G15+32*H15+64*I15+128*J15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O15" t="s">
@@ -27373,18 +27480,26 @@
         <v>13</v>
       </c>
       <c r="R15">
-        <f>+K15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S15" t="s">
         <v>12</v>
       </c>
       <c r="U15" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0630":"0",</v>
       </c>
+      <c r="Y15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA15" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0</v>
+      </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B16" s="19">
         <v>0.29166666666666702</v>
       </c>
@@ -27413,7 +27528,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="5">
-        <f>1*C16+2*D16+4*E16+8*F16+16*G16+32*H16+64*I16+128*J16</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="O16" t="s">
@@ -27426,18 +27541,26 @@
         <v>13</v>
       </c>
       <c r="R16">
-        <f>+K16</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="S16" t="s">
         <v>12</v>
       </c>
       <c r="U16" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0700":"31",</v>
       </c>
+      <c r="Y16">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="AA16" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31</v>
+      </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B17" s="18">
         <v>0.3125</v>
       </c>
@@ -27466,7 +27589,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="4">
-        <f>1*C17+2*D17+4*E17+8*F17+16*G17+32*H17+64*I17+128*J17</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="O17" t="s">
@@ -27479,18 +27602,26 @@
         <v>13</v>
       </c>
       <c r="R17">
-        <f>+K17</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="S17" t="s">
         <v>12</v>
       </c>
       <c r="U17" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0730":"31",</v>
       </c>
+      <c r="Y17">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="AA17" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31</v>
+      </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B18" s="19">
         <v>0.33333333333333298</v>
       </c>
@@ -27519,7 +27650,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="5">
-        <f>1*C18+2*D18+4*E18+8*F18+16*G18+32*H18+64*I18+128*J18</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="O18" t="s">
@@ -27532,18 +27663,26 @@
         <v>13</v>
       </c>
       <c r="R18">
-        <f>+K18</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="S18" t="s">
         <v>12</v>
       </c>
       <c r="U18" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0800":"31",</v>
       </c>
+      <c r="Y18">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="AA18" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31</v>
+      </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B19" s="18">
         <v>0.35416666666666702</v>
       </c>
@@ -27572,7 +27711,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="4">
-        <f>1*C19+2*D19+4*E19+8*F19+16*G19+32*H19+64*I19+128*J19</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O19" t="s">
@@ -27585,18 +27724,26 @@
         <v>13</v>
       </c>
       <c r="R19">
-        <f>+K19</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S19" t="s">
         <v>12</v>
       </c>
       <c r="U19" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0830":"127",</v>
       </c>
+      <c r="Y19">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA19" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127</v>
+      </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B20" s="19">
         <v>0.375</v>
       </c>
@@ -27625,7 +27772,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="5">
-        <f>1*C20+2*D20+4*E20+8*F20+16*G20+32*H20+64*I20+128*J20</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O20" t="s">
@@ -27638,18 +27785,26 @@
         <v>13</v>
       </c>
       <c r="R20">
-        <f>+K20</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S20" t="s">
         <v>12</v>
       </c>
       <c r="U20" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0900":"127",</v>
       </c>
+      <c r="Y20">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA20" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127</v>
+      </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B21" s="18">
         <v>0.39583333333333298</v>
       </c>
@@ -27678,7 +27833,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="4">
-        <f>1*C21+2*D21+4*E21+8*F21+16*G21+32*H21+64*I21+128*J21</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O21" t="s">
@@ -27691,18 +27846,26 @@
         <v>13</v>
       </c>
       <c r="R21">
-        <f>+K21</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S21" t="s">
         <v>12</v>
       </c>
       <c r="U21" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "0930":"127",</v>
       </c>
+      <c r="Y21">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA21" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127</v>
+      </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B22" s="19">
         <v>0.41666666666666702</v>
       </c>
@@ -27731,7 +27894,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="5">
-        <f>1*C22+2*D22+4*E22+8*F22+16*G22+32*H22+64*I22+128*J22</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O22" t="s">
@@ -27744,18 +27907,26 @@
         <v>13</v>
       </c>
       <c r="R22">
-        <f>+K22</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S22" t="s">
         <v>12</v>
       </c>
       <c r="U22" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1000":"127",</v>
       </c>
+      <c r="Y22">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA22" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127</v>
+      </c>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B23" s="18">
         <v>0.4375</v>
       </c>
@@ -27784,7 +27955,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="4">
-        <f>1*C23+2*D23+4*E23+8*F23+16*G23+32*H23+64*I23+128*J23</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O23" t="s">
@@ -27797,18 +27968,26 @@
         <v>13</v>
       </c>
       <c r="R23">
-        <f>+K23</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S23" t="s">
         <v>12</v>
       </c>
       <c r="U23" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1030":"127",</v>
       </c>
+      <c r="Y23">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA23" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B24" s="19">
         <v>0.45833333333333298</v>
       </c>
@@ -27837,7 +28016,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="5">
-        <f>1*C24+2*D24+4*E24+8*F24+16*G24+32*H24+64*I24+128*J24</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O24" t="s">
@@ -27850,18 +28029,26 @@
         <v>13</v>
       </c>
       <c r="R24">
-        <f>+K24</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S24" t="s">
         <v>12</v>
       </c>
       <c r="U24" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1100":"127",</v>
       </c>
+      <c r="Y24">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA24" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B25" s="18">
         <v>0.47916666666666702</v>
       </c>
@@ -27890,7 +28077,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="4">
-        <f>1*C25+2*D25+4*E25+8*F25+16*G25+32*H25+64*I25+128*J25</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O25" t="s">
@@ -27903,18 +28090,26 @@
         <v>13</v>
       </c>
       <c r="R25">
-        <f>+K25</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S25" t="s">
         <v>12</v>
       </c>
       <c r="U25" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1130":"127",</v>
       </c>
+      <c r="Y25">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA25" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B26" s="19">
         <v>0.5</v>
       </c>
@@ -27943,7 +28138,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="5">
-        <f>1*C26+2*D26+4*E26+8*F26+16*G26+32*H26+64*I26+128*J26</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O26" t="s">
@@ -27956,18 +28151,26 @@
         <v>13</v>
       </c>
       <c r="R26">
-        <f>+K26</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S26" t="s">
         <v>12</v>
       </c>
       <c r="U26" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1200":"127",</v>
       </c>
+      <c r="Y26">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA26" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B27" s="18">
         <v>0.52083333333333304</v>
       </c>
@@ -27996,7 +28199,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="4">
-        <f>1*C27+2*D27+4*E27+8*F27+16*G27+32*H27+64*I27+128*J27</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O27" t="s">
@@ -28009,18 +28212,26 @@
         <v>13</v>
       </c>
       <c r="R27">
-        <f>+K27</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S27" t="s">
         <v>12</v>
       </c>
       <c r="U27" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1230":"127",</v>
       </c>
+      <c r="Y27">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA27" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B28" s="19">
         <v>0.54166666666666696</v>
       </c>
@@ -28049,7 +28260,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="5">
-        <f>1*C28+2*D28+4*E28+8*F28+16*G28+32*H28+64*I28+128*J28</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="O28" t="s">
@@ -28062,18 +28273,26 @@
         <v>13</v>
       </c>
       <c r="R28">
-        <f>+K28</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="S28" t="s">
         <v>12</v>
       </c>
       <c r="U28" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1300":"95",</v>
       </c>
+      <c r="Y28">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="AA28" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95</v>
+      </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B29" s="18">
         <v>0.5625</v>
       </c>
@@ -28102,7 +28321,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="4">
-        <f>1*C29+2*D29+4*E29+8*F29+16*G29+32*H29+64*I29+128*J29</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="O29" t="s">
@@ -28115,18 +28334,26 @@
         <v>13</v>
       </c>
       <c r="R29">
-        <f>+K29</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="S29" t="s">
         <v>12</v>
       </c>
       <c r="U29" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1330":"95",</v>
       </c>
+      <c r="Y29">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="AA29" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95</v>
+      </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B30" s="19">
         <v>0.58333333333333304</v>
       </c>
@@ -28155,7 +28382,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="5">
-        <f>1*C30+2*D30+4*E30+8*F30+16*G30+32*H30+64*I30+128*J30</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="O30" t="s">
@@ -28168,18 +28395,26 @@
         <v>13</v>
       </c>
       <c r="R30">
-        <f>+K30</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="S30" t="s">
         <v>12</v>
       </c>
       <c r="U30" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1400":"95",</v>
       </c>
+      <c r="Y30">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="AA30" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95</v>
+      </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B31" s="18">
         <v>0.60416666666666696</v>
       </c>
@@ -28208,7 +28443,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="4">
-        <f>1*C31+2*D31+4*E31+8*F31+16*G31+32*H31+64*I31+128*J31</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="O31" t="s">
@@ -28221,18 +28456,26 @@
         <v>13</v>
       </c>
       <c r="R31">
-        <f>+K31</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="S31" t="s">
         <v>12</v>
       </c>
       <c r="U31" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1430":"95",</v>
       </c>
+      <c r="Y31">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="AA31" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95</v>
+      </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B32" s="19">
         <v>0.625</v>
       </c>
@@ -28261,7 +28504,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="5">
-        <f>1*C32+2*D32+4*E32+8*F32+16*G32+32*H32+64*I32+128*J32</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O32" t="s">
@@ -28274,18 +28517,26 @@
         <v>13</v>
       </c>
       <c r="R32">
-        <f>+K32</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S32" t="s">
         <v>12</v>
       </c>
       <c r="U32" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1500":"127",</v>
       </c>
+      <c r="Y32">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA32" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127</v>
+      </c>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B33" s="18">
         <v>0.64583333333333304</v>
       </c>
@@ -28314,7 +28565,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="4">
-        <f>1*C33+2*D33+4*E33+8*F33+16*G33+32*H33+64*I33+128*J33</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O33" t="s">
@@ -28327,18 +28578,26 @@
         <v>13</v>
       </c>
       <c r="R33">
-        <f>+K33</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S33" t="s">
         <v>12</v>
       </c>
       <c r="U33" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1530":"127",</v>
       </c>
+      <c r="Y33">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA33" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127</v>
+      </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B34" s="19">
         <v>0.66666666666666696</v>
       </c>
@@ -28367,7 +28626,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="5">
-        <f>1*C34+2*D34+4*E34+8*F34+16*G34+32*H34+64*I34+128*J34</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O34" t="s">
@@ -28380,18 +28639,26 @@
         <v>13</v>
       </c>
       <c r="R34">
-        <f>+K34</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S34" t="s">
         <v>12</v>
       </c>
       <c r="U34" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1600":"127",</v>
       </c>
+      <c r="Y34">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA34" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127</v>
+      </c>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B35" s="18">
         <v>0.6875</v>
       </c>
@@ -28420,7 +28687,7 @@
         <v>0</v>
       </c>
       <c r="K35" s="4">
-        <f>1*C35+2*D35+4*E35+8*F35+16*G35+32*H35+64*I35+128*J35</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O35" t="s">
@@ -28433,18 +28700,26 @@
         <v>13</v>
       </c>
       <c r="R35">
-        <f>+K35</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S35" t="s">
         <v>12</v>
       </c>
       <c r="U35" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1630":"127",</v>
       </c>
+      <c r="Y35">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA35" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127</v>
+      </c>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B36" s="19">
         <v>0.70833333333333304</v>
       </c>
@@ -28473,7 +28748,7 @@
         <v>0</v>
       </c>
       <c r="K36" s="5">
-        <f>1*C36+2*D36+4*E36+8*F36+16*G36+32*H36+64*I36+128*J36</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O36" t="s">
@@ -28486,18 +28761,26 @@
         <v>13</v>
       </c>
       <c r="R36">
-        <f>+K36</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S36" t="s">
         <v>12</v>
       </c>
       <c r="U36" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1700":"127",</v>
       </c>
+      <c r="Y36">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA36" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B37" s="18">
         <v>0.72916666666666696</v>
       </c>
@@ -28526,7 +28809,7 @@
         <v>0</v>
       </c>
       <c r="K37" s="4">
-        <f>1*C37+2*D37+4*E37+8*F37+16*G37+32*H37+64*I37+128*J37</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O37" t="s">
@@ -28539,18 +28822,26 @@
         <v>13</v>
       </c>
       <c r="R37">
-        <f>+K37</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S37" t="s">
         <v>12</v>
       </c>
       <c r="U37" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1730":"127",</v>
       </c>
+      <c r="Y37">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA37" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B38" s="19">
         <v>0.75</v>
       </c>
@@ -28579,7 +28870,7 @@
         <v>0</v>
       </c>
       <c r="K38" s="5">
-        <f>1*C38+2*D38+4*E38+8*F38+16*G38+32*H38+64*I38+128*J38</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O38" t="s">
@@ -28592,18 +28883,26 @@
         <v>13</v>
       </c>
       <c r="R38">
-        <f>+K38</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S38" t="s">
         <v>12</v>
       </c>
       <c r="U38" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1800":"127",</v>
       </c>
+      <c r="Y38">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA38" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B39" s="18">
         <v>0.77083333333333304</v>
       </c>
@@ -28632,7 +28931,7 @@
         <v>0</v>
       </c>
       <c r="K39" s="4">
-        <f>1*C39+2*D39+4*E39+8*F39+16*G39+32*H39+64*I39+128*J39</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O39" t="s">
@@ -28645,18 +28944,26 @@
         <v>13</v>
       </c>
       <c r="R39">
-        <f>+K39</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S39" t="s">
         <v>12</v>
       </c>
       <c r="U39" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1830":"127",</v>
       </c>
+      <c r="Y39">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA39" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B40" s="19">
         <v>0.79166666666666696</v>
       </c>
@@ -28685,7 +28992,7 @@
         <v>0</v>
       </c>
       <c r="K40" s="5">
-        <f>1*C40+2*D40+4*E40+8*F40+16*G40+32*H40+64*I40+128*J40</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O40" t="s">
@@ -28698,18 +29005,26 @@
         <v>13</v>
       </c>
       <c r="R40">
-        <f>+K40</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S40" t="s">
         <v>12</v>
       </c>
       <c r="U40" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1900":"127",</v>
       </c>
+      <c r="Y40">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA40" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B41" s="18">
         <v>0.8125</v>
       </c>
@@ -28738,7 +29053,7 @@
         <v>0</v>
       </c>
       <c r="K41" s="4">
-        <f>1*C41+2*D41+4*E41+8*F41+16*G41+32*H41+64*I41+128*J41</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O41" t="s">
@@ -28751,18 +29066,26 @@
         <v>13</v>
       </c>
       <c r="R41">
-        <f>+K41</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S41" t="s">
         <v>12</v>
       </c>
       <c r="U41" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "1930":"127",</v>
       </c>
+      <c r="Y41">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA41" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B42" s="19">
         <v>0.83333333333333304</v>
       </c>
@@ -28791,7 +29114,7 @@
         <v>0</v>
       </c>
       <c r="K42" s="5">
-        <f>1*C42+2*D42+4*E42+8*F42+16*G42+32*H42+64*I42+128*J42</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O42" t="s">
@@ -28804,18 +29127,26 @@
         <v>13</v>
       </c>
       <c r="R42">
-        <f>+K42</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S42" t="s">
         <v>12</v>
       </c>
       <c r="U42" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "2000":"127",</v>
       </c>
+      <c r="Y42">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA42" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B43" s="18">
         <v>0.85416666666666696</v>
       </c>
@@ -28844,7 +29175,7 @@
         <v>0</v>
       </c>
       <c r="K43" s="4">
-        <f>1*C43+2*D43+4*E43+8*F43+16*G43+32*H43+64*I43+128*J43</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O43" t="s">
@@ -28857,18 +29188,26 @@
         <v>13</v>
       </c>
       <c r="R43">
-        <f>+K43</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S43" t="s">
         <v>12</v>
       </c>
       <c r="U43" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "2030":"127",</v>
       </c>
+      <c r="Y43">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA43" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B44" s="19">
         <v>0.875</v>
       </c>
@@ -28897,7 +29236,7 @@
         <v>0</v>
       </c>
       <c r="K44" s="5">
-        <f>1*C44+2*D44+4*E44+8*F44+16*G44+32*H44+64*I44+128*J44</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O44" t="s">
@@ -28910,18 +29249,26 @@
         <v>13</v>
       </c>
       <c r="R44">
-        <f>+K44</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S44" t="s">
         <v>12</v>
       </c>
       <c r="U44" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "2100":"127",</v>
       </c>
+      <c r="Y44">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA44" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B45" s="18">
         <v>0.89583333333333304</v>
       </c>
@@ -28950,7 +29297,7 @@
         <v>0</v>
       </c>
       <c r="K45" s="4">
-        <f>1*C45+2*D45+4*E45+8*F45+16*G45+32*H45+64*I45+128*J45</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O45" t="s">
@@ -28963,18 +29310,26 @@
         <v>13</v>
       </c>
       <c r="R45">
-        <f>+K45</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S45" t="s">
         <v>12</v>
       </c>
       <c r="U45" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "2130":"127",</v>
       </c>
+      <c r="Y45">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA45" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127|127|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B46" s="19">
         <v>0.91666666666666696</v>
       </c>
@@ -29003,7 +29358,7 @@
         <v>0</v>
       </c>
       <c r="K46" s="5">
-        <f>1*C46+2*D46+4*E46+8*F46+16*G46+32*H46+64*I46+128*J46</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O46" t="s">
@@ -29016,18 +29371,26 @@
         <v>13</v>
       </c>
       <c r="R46">
-        <f>+K46</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S46" t="s">
         <v>12</v>
       </c>
       <c r="U46" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "2200":"127",</v>
       </c>
+      <c r="Y46">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA46" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B47" s="18">
         <v>0.9375</v>
       </c>
@@ -29056,7 +29419,7 @@
         <v>0</v>
       </c>
       <c r="K47" s="4">
-        <f>1*C47+2*D47+4*E47+8*F47+16*G47+32*H47+64*I47+128*J47</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O47" t="s">
@@ -29069,18 +29432,26 @@
         <v>13</v>
       </c>
       <c r="R47">
-        <f>+K47</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S47" t="s">
         <v>12</v>
       </c>
       <c r="U47" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "2230":"127",</v>
       </c>
+      <c r="Y47">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA47" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B48" s="19">
         <v>0.95833333333333304</v>
       </c>
@@ -29109,7 +29480,7 @@
         <v>0</v>
       </c>
       <c r="K48" s="5">
-        <f>1*C48+2*D48+4*E48+8*F48+16*G48+32*H48+64*I48+128*J48</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O48" t="s">
@@ -29122,18 +29493,26 @@
         <v>13</v>
       </c>
       <c r="R48">
-        <f>+K48</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S48" t="s">
         <v>12</v>
       </c>
       <c r="U48" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "2300":"127",</v>
       </c>
+      <c r="Y48">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA48" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="49" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="20">
         <v>0.97916666666666696</v>
       </c>
@@ -29162,7 +29541,7 @@
         <v>0</v>
       </c>
       <c r="K49" s="7">
-        <f>1*C49+2*D49+4*E49+8*F49+16*G49+32*H49+64*I49+128*J49</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="O49" t="s">
@@ -29175,20 +29554,33 @@
         <v>13</v>
       </c>
       <c r="R49">
-        <f>+K49</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="S49" t="s">
         <v>11</v>
       </c>
       <c r="U49" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">  "2330":"127"</v>
       </c>
+      <c r="Y49">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="AA49" t="str">
+        <f t="shared" si="4"/>
+        <v>0|0|0|0|0|0|0|0|0|0|0|0|0|0|31|31|31|127|127|127|127|127|127|127|127|127|95|95|95|95|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127|127</v>
+      </c>
     </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:27" x14ac:dyDescent="0.25">
       <c r="U50" s="21" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="AA51" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>